<commit_message>
fix: user import issues
--bug=1054952 --user=王旭 【系统】组织架构-通过上传文件方式导入员工失败 https://www.tapd.cn/34675357/s/1688443
</commit_message>
<xml_diff>
--- a/frontend/packages/web/public/templates/user_import_cn.xlsx
+++ b/frontend/packages/web/public/templates/user_import_cn.xlsx
@@ -1,95 +1,325 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3 xr6 xr10 x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\crm\cordys-crm\frontend\packages\web\public\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA22542-615A-47B2-B5D3-F66443174E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="15800" windowWidth="28040" xWindow="4240" yWindow="640"/>
+    <workbookView xWindow="6570" yWindow="1965" windowWidth="30750" windowHeight="17955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcMode="auto"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>admin</author>
+  </authors>
+  <commentList>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{3D26D5F8-EBE9-4125-BB65-572153576E39}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>XX公司/XX事业部/研发部</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{30879F9F-12C1-4B67-96D9-25BD9685AD9B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>员工类型：正式/实习/外包</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
-    <t/>
-    <r>
-      <rPr>
-        <sz val="9.75"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>1、Excel中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9.75"/>
-        <color rgb="FFF54A45"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>红色</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.75"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>字段为</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9.75"/>
-        <color rgb="FFF54A45"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>必填</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.75"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">字段，黑色字段为选填字段
-2、上下级部门间用‘/’隔开，且从最上级部门开始，例如"XX公司/XX事业部/研发部"。</t>
-    </r>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>填写须知：</t>
+  </si>
+  <si>
+    <t>工号</t>
+  </si>
+  <si>
+    <t>姓名</t>
+  </si>
+  <si>
+    <t>性别</t>
+  </si>
+  <si>
+    <t>职位</t>
+  </si>
+  <si>
+    <t>手机号</t>
+  </si>
+  <si>
+    <t>邮箱</t>
+  </si>
+  <si>
+    <t>直属上级</t>
+  </si>
+  <si>
+    <t>工作城市</t>
+  </si>
+  <si>
+    <t>员工类型</t>
+  </si>
+  <si>
+    <t>部门</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、不能再</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Excel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>中对成员信息类别进行增加、修改、删除</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Excel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>中红色字段为必填字段，黑色字段为选填字段</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、上下级部门间用‘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>/’</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>隔开，且从最上级部门开始，例如</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"XX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>公司</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>/XX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>事业部</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>研发部</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.75"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.75"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.75"/>
+      <color rgb="FFF54A45"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -98,29 +328,50 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="9.75"/>
-      <color rgb="FFF54A45"/>
-      <name val="Calibri"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.75"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9.75"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none">
-        <fgColor/>
-        <bgColor/>
-      </patternFill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor/>
-        <bgColor/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="4">
@@ -154,27 +405,33 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -187,7 +444,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -482,25 +739,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3 xr6 xr10 x15">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <outlinePr summaryBelow="false" summaryRight="false"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView showGridLines="true" tabSelected="true" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14" defaultRowHeight="19"/>
+  <sheetFormatPr defaultColWidth="14" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" max="1" min="1" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="3" min="3" style="0" width="14"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="true" ht="19" r="1">
-      <c r="A1" s="1" t="str">
-        <v>填写须知：</v>
+    <row r="1" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -512,56 +769,58 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row customHeight="true" ht="37" r="2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:10" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="str">
-        <v>工号</v>
-      </c>
-      <c r="B3" s="3" t="str">
-        <v>姓名</v>
-      </c>
-      <c r="C3" s="1" t="str">
-        <v>性别</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <v>部门</v>
-      </c>
-      <c r="E3" s="1" t="str">
-        <v>职位</v>
-      </c>
-      <c r="F3" s="3" t="str">
-        <v>手机号</v>
-      </c>
-      <c r="G3" s="3" t="str">
-        <v>邮箱</v>
-      </c>
-      <c r="H3" s="1" t="str">
-        <v>直属上级</v>
-      </c>
-      <c r="I3" s="1" t="str">
-        <v>工作城市</v>
-      </c>
-      <c r="J3" s="1" t="str">
-        <v>员工类型</v>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells>
+  <mergeCells count="1">
     <mergeCell ref="A2:J2"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: refactor user import
</commit_message>
<xml_diff>
--- a/frontend/packages/web/public/templates/user_import_cn.xlsx
+++ b/frontend/packages/web/public/templates/user_import_cn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\crm\cordys-crm\frontend\packages\web\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA22542-615A-47B2-B5D3-F66443174E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BDC5C1-8409-454F-AE6D-F4A8DCE290F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6570" yWindow="1965" windowWidth="30750" windowHeight="17955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6675" yWindow="1800" windowWidth="30750" windowHeight="17955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,21 +30,6 @@
     <author>admin</author>
   </authors>
   <commentList>
-    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{3D26D5F8-EBE9-4125-BB65-572153576E39}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>XX公司/XX事业部/研发部</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="J3" authorId="0" shapeId="0" xr:uid="{30879F9F-12C1-4B67-96D9-25BD9685AD9B}">
       <text>
         <r>
@@ -346,14 +331,6 @@
     </font>
     <font>
       <sz val="9.75"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9.75"/>
       <color rgb="FF000000"/>
       <name val="等线"/>
       <family val="2"/>
@@ -364,6 +341,14 @@
       <color rgb="FF000000"/>
       <name val="等线"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.75"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -417,14 +402,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -746,7 +731,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -770,18 +755,18 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -793,7 +778,7 @@
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">

</xml_diff>